<commit_message>
added drag-drop, changed layout+logic
to-do
- goal configuration ends game
- make some moves invalid in drag-drop
- shapes instead of light/dark
</commit_message>
<xml_diff>
--- a/helping-game/tableconfiguration.xlsx
+++ b/helping-game/tableconfiguration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhilashakumar/helping-behavior-game/games/helping-game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA1D4F3A-9E61-D740-B781-A794399EB055}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACEBD26-21BC-C64E-9E9F-8C309CEA1367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16100" xr2:uid="{BC9B4203-94A0-5243-8CBD-CB7149E0043F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BC9B4203-94A0-5243-8CBD-CB7149E0043F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>A1</t>
   </si>
@@ -45,9 +45,6 @@
     <t>A3</t>
   </si>
   <si>
-    <t>white</t>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
@@ -64,6 +61,15 @@
   </si>
   <si>
     <t>C3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>C4</t>
   </si>
 </sst>
 </file>
@@ -87,10 +93,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -99,9 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -421,7 +439,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +457,7 @@
       <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="2">
         <v>3</v>
       </c>
       <c r="E1" s="1">
@@ -451,7 +469,7 @@
       <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1" s="2">
         <v>7</v>
       </c>
       <c r="I1" s="1">
@@ -477,7 +495,7 @@
       <c r="C2" s="1">
         <v>14</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>15</v>
       </c>
       <c r="E2" s="1">
@@ -489,7 +507,7 @@
       <c r="G2" s="1">
         <v>18</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>19</v>
       </c>
       <c r="I2" s="1">
@@ -515,7 +533,7 @@
       <c r="C3" s="1">
         <v>26</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>27</v>
       </c>
       <c r="E3" s="1">
@@ -527,7 +545,7 @@
       <c r="G3" s="1">
         <v>30</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>31</v>
       </c>
       <c r="I3" s="1">
@@ -553,32 +571,32 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>